<commit_message>
updated excel sheets for github as source
</commit_message>
<xml_diff>
--- a/github-ado/github-to-azure.xlsx
+++ b/github-ado/github-to-azure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varsharma\Desktop\version control excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abharamagoudar\Desktop\api\github\SCM-Migration-DEMO\github-ado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08BDB07-0E15-4726-8A39-6AA7C4516C7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4F7D1A-BF58-49F0-AE32-2118F5985C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>sr</t>
   </si>
@@ -36,23 +36,47 @@
     <t>repo_name_to_import</t>
   </si>
   <si>
-    <t>devops-TEKsystems/test</t>
-  </si>
-  <si>
     <t>azure_target_namespace</t>
   </si>
   <si>
-    <t>varun1699sharma</t>
-  </si>
-  <si>
-    <t>online-test</t>
+    <t>code-migration</t>
+  </si>
+  <si>
+    <t>casaplotms </t>
+  </si>
+  <si>
+    <t>casa-build-utils </t>
+  </si>
+  <si>
+    <t>casashell</t>
+  </si>
+  <si>
+    <t>casaaddons </t>
+  </si>
+  <si>
+    <t>cartavis </t>
+  </si>
+  <si>
+    <t>carta-casacore</t>
+  </si>
+  <si>
+    <t>casa-asap </t>
+  </si>
+  <si>
+    <t>almatasks </t>
+  </si>
+  <si>
+    <t>app-n-pak </t>
+  </si>
+  <si>
+    <t>repo-migartion/git-project</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +88,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,14 +124,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -372,20 +415,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="59.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="59.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,21 +439,133 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>